<commit_message>
define a new class api_request
</commit_message>
<xml_diff>
--- a/data/api.xlsx
+++ b/data/api.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="接口" sheetId="1" r:id="rId1"/>
+    <sheet name="登录" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,6 +35,22 @@
   </si>
   <si>
     <t>接口参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户登录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/account/login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -381,15 +397,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -407,6 +425,23 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -420,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>